<commit_message>
backend gestion utilisateurs(login, inscription) sans envoyer mail, sans generer token
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="54">
   <si>
     <t>Catégorie</t>
   </si>
@@ -566,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +621,7 @@
         <v>120</v>
       </c>
       <c r="E2" s="4">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -640,7 +640,7 @@
         <v>120</v>
       </c>
       <c r="E3" s="4">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -659,10 +659,10 @@
         <v>60</v>
       </c>
       <c r="E4" s="4">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F4" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -679,8 +679,12 @@
       <c r="D5" s="4">
         <v>60</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="4">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4">
+        <v>30</v>
+      </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -696,8 +700,12 @@
       <c r="D6" s="4">
         <v>30</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="4">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -714,9 +722,11 @@
         <v>60</v>
       </c>
       <c r="E7" s="4">
-        <v>20</v>
-      </c>
-      <c r="F7" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="F7" s="4">
+        <v>10</v>
+      </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -749,8 +759,12 @@
       <c r="D9" s="4">
         <v>15</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="4">
+        <v>15</v>
+      </c>
+      <c r="F9" s="4">
+        <v>10</v>
+      </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -800,8 +814,12 @@
       <c r="D12" s="4">
         <v>60</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="4">
+        <v>30</v>
+      </c>
+      <c r="F12" s="4">
+        <v>30</v>
+      </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1571,7 +1589,10 @@
         <f>SUM(D2:D57)</f>
         <v>1250</v>
       </c>
-      <c r="E58" s="6"/>
+      <c r="E58" s="6">
+        <f>SUM(E2:E57)</f>
+        <v>335</v>
+      </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
     </row>
@@ -1582,6 +1603,15 @@
       <c r="B60" s="3">
         <f>D58/60</f>
         <v>20.833333333333332</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="3">
+        <f>E58/60</f>
+        <v>5.583333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout footer angular, Modification login
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -569,7 +569,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,10 +680,10 @@
         <v>60</v>
       </c>
       <c r="E5" s="4">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="F5" s="4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="E58" s="6">
         <f>SUM(E2:E57)</f>
-        <v>395</v>
+        <v>465</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="B61" s="3">
         <f>E58/60</f>
-        <v>6.583333333333333</v>
+        <v>7.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>